<commit_message>
binomio de newton (complejidades)
</commit_message>
<xml_diff>
--- a/TP3-Polinomio/graficoYComplejidad.xlsx
+++ b/TP3-Polinomio/graficoYComplejidad.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laboratorios\Desktop\PrograKikeFede\ProgramacionAvanzada\TP3-Polinomio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lautaro\workspace\PrograAvanzada\repoFede\ProgramacionAvanzada\TP3-Polinomio\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Polinomio" sheetId="1" r:id="rId1"/>
     <sheet name="Complejidad" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>N</t>
   </si>
@@ -73,6 +74,33 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>crearTrianguloDePascal</t>
+  </si>
+  <si>
+    <t>combinatoriaRecursiva</t>
+  </si>
+  <si>
+    <t>n!</t>
+  </si>
+  <si>
+    <t>combinatoriaNoRecur</t>
+  </si>
+  <si>
+    <t>obtenerCoeficienteDelTerminoK</t>
+  </si>
+  <si>
+    <t>obtenerCoeficienteDelTerminoKMejorado</t>
+  </si>
+  <si>
+    <t>desarrollar</t>
+  </si>
+  <si>
+    <t>n*n!</t>
+  </si>
+  <si>
+    <t>desarrollarMejorado</t>
   </si>
 </sst>
 </file>
@@ -124,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -132,6 +160,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -829,7 +860,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1309975952"/>
@@ -891,7 +922,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1309989264"/>
@@ -934,7 +965,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -964,7 +995,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1571,7 +1602,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
@@ -1625,8 +1656,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="180627" cy="175369"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CuadroTexto 2"/>
@@ -1662,6 +1693,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1701,7 +1733,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CuadroTexto 2"/>
@@ -1759,8 +1791,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="180627" cy="175369"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="CuadroTexto 3"/>
@@ -1796,6 +1828,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1835,7 +1868,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="CuadroTexto 3"/>
@@ -1893,8 +1926,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="428514" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="CuadroTexto 4"/>
@@ -1930,6 +1963,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1978,7 +2012,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="CuadroTexto 4"/>
@@ -2019,6 +2053,478 @@
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>𝑛 log⁡𝑛</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-AR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="CuadroTexto 11"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6362700" y="209550"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="CuadroTexto 12"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6362700" y="400050"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="295275" cy="257175"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="CuadroTexto 13"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6257925" y="590550"/>
+          <a:ext cx="295275" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="180627" cy="175369"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="15" name="CuadroTexto 14"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1638300" y="209550"/>
+              <a:ext cx="180627" cy="175369"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="es-ES" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="es-ES" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑛</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="es-ES" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-AR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="15" name="CuadroTexto 14"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1638300" y="209550"/>
+              <a:ext cx="180627" cy="175369"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑛^2</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-AR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="CuadroTexto 15"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7305675" y="209550"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr/>
+          <a:endParaRPr lang="es-AR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="180627" cy="175369"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="17" name="CuadroTexto 16"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7620000" y="209550"/>
+              <a:ext cx="180627" cy="175369"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="es-ES" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="es-ES" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑛</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="es-ES" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-AR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="17" name="CuadroTexto 16"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7620000" y="209550"/>
+              <a:ext cx="180627" cy="175369"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑛^2</a:t>
               </a:r>
               <a:endParaRPr lang="es-AR" sz="1100"/>
             </a:p>
@@ -2478,58 +2984,93 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -2537,9 +3078,33 @@
         <v>15</v>
       </c>
       <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>